<commit_message>
Enhance table display for real-time posting feedback
- Revamped display_dataframe_as_table to dynamically generate color-coded tables, highlighting successful posts in green and today's scheduled posts in white, for enhanced visual clarity and immediate feedback on post statuses.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDED5417-ABDA-4064-AD27-936CF18BDC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C894B-2209-45DB-9CE6-D727243159C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="5100" windowWidth="28740" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="4130" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
   <si>
     <t>Post ID</t>
   </si>
@@ -147,6 +147,48 @@
   </si>
   <si>
     <t>img14</t>
+  </si>
+  <si>
+    <t>TestFI 12</t>
+  </si>
+  <si>
+    <t>img15</t>
+  </si>
+  <si>
+    <t>TestFI 13</t>
+  </si>
+  <si>
+    <t>img16</t>
+  </si>
+  <si>
+    <t>TestFI 14</t>
+  </si>
+  <si>
+    <t>img17</t>
+  </si>
+  <si>
+    <t>TestFI 15</t>
+  </si>
+  <si>
+    <t>img18</t>
+  </si>
+  <si>
+    <t>TestFI 16</t>
+  </si>
+  <si>
+    <t>img19</t>
+  </si>
+  <si>
+    <t>TestFI 17</t>
+  </si>
+  <si>
+    <t>img20</t>
+  </si>
+  <si>
+    <t>TestFI 18</t>
+  </si>
+  <si>
+    <t>img21</t>
   </si>
 </sst>
 </file>
@@ -519,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -853,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="2">
-        <v>45323.576388888891</v>
+        <v>45328.832638888889</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
@@ -876,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="2">
-        <v>45325.944444444445</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -899,7 +941,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -922,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -945,7 +987,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -968,7 +1010,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -991,7 +1033,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.568749999999</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1014,9 +1056,170 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45325.945138888892</v>
+        <v>45336.652083333334</v>
       </c>
       <c r="G21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2">
+        <v>45336.652083333334</v>
+      </c>
+      <c r="G28" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create LoggerSingleton and logging_lock.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C894B-2209-45DB-9CE6-D727243159C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FEF01E-2D8A-4069-B830-3D09A250128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="4130" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4123" yWindow="2486" windowWidth="28791" windowHeight="15308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
   <si>
     <t>Post ID</t>
   </si>
@@ -189,6 +189,66 @@
   </si>
   <si>
     <t>img21</t>
+  </si>
+  <si>
+    <t>TestFI 19</t>
+  </si>
+  <si>
+    <t>img22</t>
+  </si>
+  <si>
+    <t>TestFI 20</t>
+  </si>
+  <si>
+    <t>img23</t>
+  </si>
+  <si>
+    <t>TestFI 21</t>
+  </si>
+  <si>
+    <t>img24</t>
+  </si>
+  <si>
+    <t>TestFI 22</t>
+  </si>
+  <si>
+    <t>img25</t>
+  </si>
+  <si>
+    <t>TestFI 23</t>
+  </si>
+  <si>
+    <t>img26</t>
+  </si>
+  <si>
+    <t>TestFI 24</t>
+  </si>
+  <si>
+    <t>img27</t>
+  </si>
+  <si>
+    <t>TestFI 25</t>
+  </si>
+  <si>
+    <t>img28</t>
+  </si>
+  <si>
+    <t>TestFI 26</t>
+  </si>
+  <si>
+    <t>img29</t>
+  </si>
+  <si>
+    <t>TestFI 27</t>
+  </si>
+  <si>
+    <t>img30</t>
+  </si>
+  <si>
+    <t>TestFI 28</t>
+  </si>
+  <si>
+    <t>img31</t>
   </si>
 </sst>
 </file>
@@ -561,22 +621,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -625,7 +685,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -648,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -671,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -694,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -717,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -740,7 +800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -763,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -786,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -809,7 +869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -832,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -855,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -878,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -901,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -924,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -947,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -970,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -993,7 +1053,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1016,7 +1076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1039,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1056,13 +1116,13 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1079,13 +1139,13 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1102,13 +1162,13 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1125,13 +1185,13 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1148,13 +1208,13 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1171,13 +1231,13 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1194,13 +1254,13 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1217,9 +1277,239 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45336.652083333334</v>
+        <v>45337.004861111112</v>
       </c>
       <c r="G28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="2">
+        <v>45337.004861111112</v>
+      </c>
+      <c r="G38" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add enhanced job completion listener with colored console output
Implemented a new listener function `my_listener` for APScheduler jobs that provides immediate visual feedback on job execution results. This function utilizes the `rich` library to print job completion status with distinct colors: red for failures and green for successes, making it easier to monitor job outcomes at a glance. Surrounding the status messages with dashes enhances visibility in the console output.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FEF01E-2D8A-4069-B830-3D09A250128B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234E7137-C9D8-4F82-85A3-2B9C505A0738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4123" yWindow="2486" windowWidth="28791" windowHeight="15308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6790" yWindow="5860" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,20 +623,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -708,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -731,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -777,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -800,7 +800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -823,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -846,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -869,7 +869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -892,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -915,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -938,7 +938,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -961,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -984,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1116,13 +1116,13 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1139,13 +1139,13 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1162,13 +1162,13 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1185,13 +1185,13 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1208,13 +1208,13 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1231,13 +1231,13 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1254,13 +1254,13 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1277,13 +1277,13 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1300,13 +1300,13 @@
         <v>11</v>
       </c>
       <c r="F29" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1323,13 +1323,13 @@
         <v>11</v>
       </c>
       <c r="F30" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1346,13 +1346,13 @@
         <v>11</v>
       </c>
       <c r="F31" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1369,13 +1369,13 @@
         <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1392,13 +1392,13 @@
         <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1415,13 +1415,13 @@
         <v>11</v>
       </c>
       <c r="F34" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1438,13 +1438,13 @@
         <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1461,13 +1461,13 @@
         <v>11</v>
       </c>
       <c r="F36" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1484,13 +1484,13 @@
         <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="2">
-        <v>45337.004861111112</v>
+        <v>45337.501388888886</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Refactor logging to ensure thread safety across the application
This commit overhauls the application's logging mechanism to enhance thread safety and simplify the codebase. Specifically, it removes the unnecessary threading lock from the logging decorator, leveraging the inherent thread safety of Python's logging module. Concurrently, it introduces a threading lock in the LoggerSingleton class to prevent race conditions during the logger instance creation process in a multithreaded environment. This dual approach streamlines logging operations while ensuring that logger instances are managed in a thread-safe manner, thereby improving both the reliability and maintainability of the logging system.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234E7137-C9D8-4F82-85A3-2B9C505A0738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23832019-C38A-42A1-BEB5-80D281045681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6790" yWindow="5860" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6790" yWindow="5510" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -623,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F21" sqref="F21:F38"/>
     </sheetView>
   </sheetViews>
@@ -1116,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -1139,7 +1139,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -1162,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -1185,7 +1185,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G24" t="s">
         <v>12</v>
@@ -1208,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -1231,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1254,7 +1254,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1277,7 +1277,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
@@ -1300,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1323,7 +1323,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1346,7 +1346,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1369,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
@@ -1392,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
@@ -1415,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G34" t="s">
         <v>12</v>
@@ -1438,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1461,7 +1461,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1484,7 +1484,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="2">
-        <v>45337.501388888886</v>
+        <v>45338.495833333334</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
feat: integrate DataHolder for state management, refactor PostExecutor, and update tests
Introduce the DataHolder class to manage DataFrame states centrally, allowing for more efficient data manipulations and updates. Refactor PostExecutor to utilize DataHolder for improved data consistency and isolation in post scheduling tasks. Update unit tests to accommodate new changes in PostExecutor, ensuring it properly interacts with DataHolder and maintains correct functionality with refreshed data setups. This integration simplifies data management, enhances maintainability, and optimizes the posting process by ensuring the use of current data across cycles.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F7CAE-6098-4E77-A87B-488250BC144D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900438F3-5DC5-44AF-B524-D0106B2C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5690" yWindow="3720" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -757,20 +757,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F16" sqref="F16:F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +799,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -825,7 +825,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -851,7 +851,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -877,7 +877,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -903,7 +903,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -929,7 +929,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -955,7 +955,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -981,7 +981,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -1189,7 +1189,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -1215,7 +1215,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -1241,7 +1241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1267,7 +1267,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1293,7 +1293,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -1319,7 +1319,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -1345,7 +1345,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -1371,7 +1371,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G24" t="s">
         <v>48</v>
@@ -1397,7 +1397,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -1423,7 +1423,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1449,7 +1449,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1475,7 +1475,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G28" t="s">
         <v>57</v>
@@ -1501,7 +1501,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G29" t="s">
         <v>57</v>
@@ -1527,7 +1527,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1553,7 +1553,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1579,7 +1579,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
@@ -1605,7 +1605,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
@@ -1631,7 +1631,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G34" t="s">
         <v>48</v>
@@ -1657,7 +1657,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1683,7 +1683,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1709,7 +1709,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
@@ -1735,7 +1735,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="2">
-        <v>45391.806944444441</v>
+        <v>45393.878472222219</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Refactor DataHolder and executors to use self.data_source
- Added self.data_source in DataHolder to replace path_file, centralizing data management within DataHolder instances.
- Refactored PostExecutor and BotManager to utilize DataHolder instead of direct file path references. This change simplifies data handling and enhances modularity.
- Updated tests to reflect changes in data handling mechanisms. This involves modifying test setups to initialize DataHolder instances with appropriate data sources instead of file paths.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900438F3-5DC5-44AF-B524-D0106B2C7475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386AB5B1-9493-44DD-9E6E-A8E44F7DC92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5690" yWindow="3720" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,7 +758,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F38"/>
+      <selection activeCell="F35" sqref="F35:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -1362,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -1388,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G24" t="s">
         <v>48</v>
@@ -1414,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -1440,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1466,7 +1466,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1492,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.951388888891</v>
       </c>
       <c r="G28" t="s">
         <v>57</v>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G29" t="s">
         <v>57</v>
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1596,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
@@ -1622,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
@@ -1648,7 +1648,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.952777777777</v>
       </c>
       <c r="G34" t="s">
         <v>48</v>
@@ -1674,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.95416666667</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1700,7 +1700,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.95416666667</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1726,7 +1726,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.95416666667</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
@@ -1752,7 +1752,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="2">
-        <v>45393.878472222219</v>
+        <v>45393.95416666667</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Major refactoring: directory and class names updated
- Renamed bot_core/posts to media to better align with its usage which involves handling media files rather than just textual posts.
- Class names updated to clarify their roles and functionalities:
  - BotProtocol, AbstractBot, AbstractAuthenticator, and MediaContent

These changes ensure the codebase is more intuitive and maintainable, with clear distinctions and responsibilities laid out through precise naming.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\PycharmProjects\SocialMediaManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0318C326-7E3D-4FC0-AA52-1DB235D4270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2EC045-63FA-41A9-9872-68F89EB6D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5690" yWindow="3720" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1886" yWindow="1886" windowWidth="24685" windowHeight="13097" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -677,22 +677,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F16" sqref="F16:F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.4609375" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -747,7 +747,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -773,7 +773,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -799,7 +799,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -825,7 +825,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -851,7 +851,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -877,7 +877,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -903,7 +903,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -929,7 +929,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -955,7 +955,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -981,7 +981,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G16" t="s">
         <v>12</v>
@@ -1111,7 +1111,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G17" t="s">
         <v>12</v>
@@ -1137,7 +1137,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G18" t="s">
         <v>12</v>
@@ -1163,7 +1163,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1189,7 +1189,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
@@ -1215,7 +1215,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G21" t="s">
         <v>12</v>
@@ -1241,7 +1241,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
@@ -1267,7 +1267,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
@@ -1293,7 +1293,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G24" t="s">
         <v>48</v>
@@ -1319,7 +1319,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -1345,7 +1345,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G26" t="s">
         <v>12</v>
@@ -1371,7 +1371,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1397,7 +1397,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G28" t="s">
         <v>57</v>
@@ -1423,7 +1423,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G29" t="s">
         <v>57</v>
@@ -1449,7 +1449,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
@@ -1475,7 +1475,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1501,7 +1501,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
@@ -1527,7 +1527,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G33" t="s">
         <v>12</v>
@@ -1553,7 +1553,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G34" t="s">
         <v>48</v>
@@ -1579,7 +1579,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1605,7 +1605,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
@@ -1631,7 +1631,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>11</v>
       </c>
       <c r="F37" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
@@ -1657,7 +1657,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="2">
-        <v>45396.898611111108</v>
+        <v>45397.919444444444</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>

</xml_diff>